<commit_message>
Combine station 5 and 5b
Also some changes to the plot:
- Station_name changed
- Distance changed
</commit_message>
<xml_diff>
--- a/Figures/06_Littorina_tables.xlsx
+++ b/Figures/06_Littorina_tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5b</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
@@ -511,11 +508,15 @@
         <v>0</v>
       </c>
       <c r="D4"/>
-      <c r="E4"/>
+      <c r="E4" t="n">
+        <v>35.7</v>
+      </c>
       <c r="F4"/>
-      <c r="G4"/>
+      <c r="G4" t="n">
+        <v>243</v>
+      </c>
       <c r="H4" t="n">
-        <v>96.7</v>
+        <v>120.35</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -532,21 +533,33 @@
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5"/>
+      <c r="D5" t="n">
+        <v>148</v>
+      </c>
       <c r="E5" t="n">
-        <v>35.7</v>
-      </c>
-      <c r="F5"/>
+        <v>31.3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>69.8</v>
+      </c>
       <c r="G5" t="n">
-        <v>243</v>
+        <v>500</v>
       </c>
       <c r="H5" t="n">
-        <v>144</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
+        <v>266</v>
+      </c>
+      <c r="I5" t="n">
+        <v>234</v>
+      </c>
+      <c r="J5" t="n">
+        <v>211</v>
+      </c>
+      <c r="K5" t="n">
+        <v>104</v>
+      </c>
+      <c r="L5" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -558,65 +571,27 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v>148</v>
-      </c>
+      <c r="D6"/>
       <c r="E6" t="n">
-        <v>31.3</v>
-      </c>
-      <c r="F6" t="n">
-        <v>69.8</v>
-      </c>
+        <v>97.7</v>
+      </c>
+      <c r="F6"/>
       <c r="G6" t="n">
-        <v>500</v>
+        <v>113</v>
       </c>
       <c r="H6" t="n">
-        <v>266</v>
+        <v>78.8</v>
       </c>
       <c r="I6" t="n">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="J6" t="n">
-        <v>211</v>
+        <v>80.7</v>
       </c>
       <c r="K6" t="n">
-        <v>104</v>
+        <v>51.4</v>
       </c>
       <c r="L6" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7" t="n">
-        <v>97.7</v>
-      </c>
-      <c r="F7"/>
-      <c r="G7" t="n">
-        <v>113</v>
-      </c>
-      <c r="H7" t="n">
-        <v>78.8</v>
-      </c>
-      <c r="I7" t="n">
-        <v>123</v>
-      </c>
-      <c r="J7" t="n">
-        <v>80.7</v>
-      </c>
-      <c r="K7" t="n">
-        <v>51.4</v>
-      </c>
-      <c r="L7" t="n">
         <v>29</v>
       </c>
     </row>
@@ -654,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -728,10 +703,14 @@
       <c r="B4" t="n">
         <v>1.67</v>
       </c>
-      <c r="C4"/>
-      <c r="D4"/>
+      <c r="C4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.4</v>
+      </c>
       <c r="E4" t="n">
-        <v>0.27</v>
+        <v>0.52</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -748,86 +727,61 @@
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="n">
+        <v>3.05</v>
+      </c>
       <c r="C5" t="n">
-        <v>0.68</v>
+        <v>1.75</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4</v>
+        <v>1.85</v>
       </c>
       <c r="E5" t="n">
-        <v>0.87</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5"/>
-      <c r="I5"/>
+        <v>0.76</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.19</v>
+      </c>
       <c r="J5"/>
-      <c r="K5"/>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="n">
-        <v>3.05</v>
-      </c>
+      <c r="B6"/>
       <c r="C6" t="n">
-        <v>1.75</v>
+        <v>1.45</v>
       </c>
       <c r="D6" t="n">
-        <v>1.85</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>0.45</v>
       </c>
       <c r="F6" t="n">
-        <v>0.79</v>
+        <v>0.32</v>
       </c>
       <c r="G6" t="n">
-        <v>0.76</v>
+        <v>0.06</v>
       </c>
       <c r="H6" t="n">
-        <v>0.69</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.19</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I6"/>
       <c r="J6"/>
       <c r="K6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -865,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -939,10 +893,14 @@
       <c r="B4" t="n">
         <v>1.67</v>
       </c>
-      <c r="C4"/>
-      <c r="D4"/>
+      <c r="C4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.4</v>
+      </c>
       <c r="E4" t="n">
-        <v>0.27</v>
+        <v>0.52</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -959,86 +917,61 @@
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="n">
+        <v>3.05</v>
+      </c>
       <c r="C5" t="n">
-        <v>0.68</v>
+        <v>1.75</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4</v>
+        <v>1.85</v>
       </c>
       <c r="E5" t="n">
-        <v>0.87</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5"/>
-      <c r="I5"/>
+        <v>0.76</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.19</v>
+      </c>
       <c r="J5"/>
-      <c r="K5"/>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="n">
-        <v>3.05</v>
-      </c>
+      <c r="B6"/>
       <c r="C6" t="n">
-        <v>1.75</v>
+        <v>1.45</v>
       </c>
       <c r="D6" t="n">
-        <v>1.85</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>0.45</v>
       </c>
       <c r="F6" t="n">
-        <v>0.79</v>
+        <v>0.32</v>
       </c>
       <c r="G6" t="n">
-        <v>0.76</v>
+        <v>0.06</v>
       </c>
       <c r="H6" t="n">
-        <v>0.69</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.19</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I6"/>
       <c r="J6"/>
       <c r="K6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1076,7 +1009,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1111,10 +1044,14 @@
       <c r="B3" t="n">
         <v>2.01</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
       <c r="E3" t="n">
-        <v>5.83</v>
+        <v>5.22</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -1126,75 +1063,55 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" t="n">
+        <v>5.25</v>
+      </c>
       <c r="C4" t="n">
-        <v>3.11</v>
+        <v>3.98</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>6.24</v>
       </c>
       <c r="E4" t="n">
-        <v>4.92</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
+        <v>4.88</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3.3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="n">
-        <v>5.25</v>
-      </c>
+      <c r="B5"/>
       <c r="C5" t="n">
-        <v>3.98</v>
+        <v>5.5</v>
       </c>
       <c r="D5" t="n">
-        <v>6.24</v>
+        <v>5.6</v>
       </c>
       <c r="E5" t="n">
-        <v>4.88</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
-        <v>4.62</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2.57</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6"/>
-      <c r="C6" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="E6" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" t="n">
         <v>5.9</v>
       </c>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Combine statins 5 + 5b for more figures
</commit_message>
<xml_diff>
--- a/Figures/06_Littorina_tables.xlsx
+++ b/Figures/06_Littorina_tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -26,6 +26,9 @@
     <t xml:space="preserve">TBT_flag</t>
   </si>
   <si>
+    <t xml:space="preserve">Station_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">2005</t>
   </si>
   <si>
@@ -59,16 +62,31 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference station (5.5 km)</t>
+  </si>
+  <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
+    <t xml:space="preserve">Outer Vikkilen (2.5 km)</t>
+  </si>
+  <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
+    <t xml:space="preserve">Skjeviga (0.1 km)</t>
+  </si>
+  <si>
     <t xml:space="preserve">6</t>
   </si>
   <si>
+    <t xml:space="preserve">Shipyard (0 km)</t>
+  </si>
+  <si>
     <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inner Vikkilen (0.5 km)</t>
   </si>
   <si>
     <t xml:space="preserve">2012</t>
@@ -440,158 +458,176 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="H2" t="n">
+      <c r="H2"/>
+      <c r="I2" t="n">
         <v>5</v>
       </c>
-      <c r="I2"/>
       <c r="J2"/>
-      <c r="K2" t="n">
+      <c r="K2"/>
+      <c r="L2" t="n">
         <v>1</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>1.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
-      <c r="D3"/>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
-      <c r="H3" t="n">
+      <c r="H3"/>
+      <c r="I3" t="n">
         <v>30.4</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>31</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>34.7</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>11.6</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>6.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="D4"/>
-      <c r="E4" t="n">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4" t="n">
         <v>35.7</v>
       </c>
-      <c r="F4"/>
-      <c r="G4" t="n">
+      <c r="G4"/>
+      <c r="H4" t="n">
         <v>243</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>120.35</v>
       </c>
-      <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
+      <c r="M4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="n">
         <v>148</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>31.3</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>69.8</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>500</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>266</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>234</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>211</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>104</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6"/>
-      <c r="E6" t="n">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6" t="n">
         <v>97.7</v>
       </c>
-      <c r="F6"/>
-      <c r="G6" t="n">
+      <c r="G6"/>
+      <c r="H6" t="n">
         <v>113</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>78.8</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>123</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>80.7</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>51.4</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>29</v>
       </c>
     </row>
@@ -614,39 +650,39 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -667,7 +703,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="n">
         <v>0.44</v>
@@ -698,7 +734,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
         <v>1.67</v>
@@ -725,7 +761,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>3.05</v>
@@ -758,7 +794,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="n">
@@ -804,39 +840,39 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -857,7 +893,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="n">
         <v>0.44</v>
@@ -888,7 +924,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
         <v>1.67</v>
@@ -915,7 +951,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>3.05</v>
@@ -948,7 +984,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="n">
@@ -994,36 +1030,36 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" t="n">
         <v>4.4</v>
@@ -1039,7 +1075,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="n">
         <v>2.01</v>
@@ -1061,7 +1097,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B4" t="n">
         <v>5.25</v>
@@ -1093,7 +1129,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="n">

</xml_diff>

<commit_message>
Update of 06 scripts
</commit_message>
<xml_diff>
--- a/Figures/06_Littorina_tables.xlsx
+++ b/Figures/06_Littorina_tables.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -14,11 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Station</t>
   </si>
   <si>
+    <t xml:space="preserve">2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009</t>
+  </si>
+  <si>
     <t xml:space="preserve">2010</t>
   </si>
   <si>
@@ -44,6 +53,24 @@
   </si>
   <si>
     <t xml:space="preserve">2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
   </si>
   <si>
     <t xml:space="preserve">71G</t>
@@ -52,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -371,12 +398,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -409,32 +436,218 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
+      <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -443,12 +656,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -481,32 +694,218 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
+      <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -515,46 +914,252 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5.24</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>